<commit_message>
restructuring of application categories
</commit_message>
<xml_diff>
--- a/applications.xlsx
+++ b/applications.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nasser\Documents\personal\frontend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\personal\frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="9630" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="9630" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="High" sheetId="2" r:id="rId2"/>
-    <sheet name="requirements" sheetId="3" r:id="rId3"/>
+    <sheet name="very high" sheetId="4" r:id="rId2"/>
+    <sheet name="uni-assist" sheetId="2" r:id="rId3"/>
+    <sheet name="requirements" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="152">
   <si>
     <t>Course</t>
   </si>
@@ -125,9 +126,6 @@
   </si>
   <si>
     <t>http://www.uni-bamberg.de/en/ma-isosysc ,https://www.uni-bamberg.de/en/studies/non-exchange-students-masters-degree/online-application-form/</t>
-  </si>
-  <si>
-    <t>Master of Science in Web and Data Science</t>
   </si>
   <si>
     <t>Web and Data Science (MSc)</t>
@@ -457,19 +455,37 @@
     <t>Bachelors(2.5 or better),TOEFL iBT 90 (Internet-based), German A1 Certificate,Bachelor's thesis, Proof of internship/work(18 months minimum)</t>
   </si>
   <si>
-    <t>Master of Science in Quantitative Finance</t>
-  </si>
-  <si>
-    <t>Bachelors(2.5 or better),TOEFL iBT 90 (Internet-based), Proof of internship/work in finance(18 months minimum)</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>http://www.uni-assist.de/en/ ,https://www.wiso.uni-kiel.de/en/study/master/quantitative-finance</t>
-  </si>
-  <si>
     <t>REQUIREMENT</t>
+  </si>
+  <si>
+    <t>TOEFL(ibt  90+)</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>Letter of Motivation</t>
+  </si>
+  <si>
+    <t>Get it before end of March</t>
+  </si>
+  <si>
+    <t>Clear for transcript before end of March</t>
+  </si>
+  <si>
+    <t>Consult Mo on how to structure it before end of March</t>
+  </si>
+  <si>
+    <t>Research and craft it carefully before end of March</t>
+  </si>
+  <si>
+    <t>COMMENT</t>
+  </si>
+  <si>
+    <t>Proof of Degree in English</t>
+  </si>
+  <si>
+    <t>Scientific Essay</t>
   </si>
 </sst>
 </file>
@@ -886,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="I25" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,89 +950,95 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
+      <c r="A2" t="s">
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2">
         <v>11049</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
+      <c r="A3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
-        <v>23</v>
+      <c r="E3" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="F3" s="2">
-        <v>11049</v>
+        <v>42156</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
         <v>17</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F4" s="2">
-        <v>11049</v>
+        <v>42125</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -1024,28 +1046,28 @@
       <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="2">
-        <v>42156</v>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>34</v>
+      <c r="A6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -1054,33 +1076,33 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="F6" s="2">
-        <v>42125</v>
+        <v>11383</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H6" t="s">
         <v>10</v>
       </c>
       <c r="I6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
       </c>
       <c r="F7" s="2">
         <v>42125</v>
@@ -1089,18 +1111,18 @@
         <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>41</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -1109,7 +1131,7 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="F8" s="2">
         <v>42125</v>
@@ -1118,18 +1140,18 @@
         <v>9</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>42</v>
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>44</v>
+      <c r="A9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -1138,39 +1160,36 @@
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>45</v>
+        <v>66</v>
+      </c>
+      <c r="F9" s="2">
+        <v>42125</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
         <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
+      <c r="A10" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="F10" s="2">
-        <v>11383</v>
+        <v>43891</v>
       </c>
       <c r="G10" t="s">
         <v>25</v>
@@ -1179,24 +1198,21 @@
         <v>10</v>
       </c>
       <c r="I10" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
+      <c r="A11" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="F11" s="2">
         <v>11383</v>
@@ -1205,192 +1221,189 @@
         <v>25</v>
       </c>
       <c r="H11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>77</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="2">
         <v>42125</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="H12" t="s">
         <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>58</v>
+      <c r="A13" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" s="2">
+        <v>11444</v>
+      </c>
+      <c r="G13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="2">
+        <v>11383</v>
+      </c>
+      <c r="G14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="2">
+        <v>11049</v>
+      </c>
+      <c r="G15" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="2">
         <v>42125</v>
       </c>
-      <c r="G13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="2">
+      <c r="G16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="2">
         <v>42125</v>
       </c>
-      <c r="G14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="11" t="s">
+      <c r="G17" t="s">
         <v>64</v>
       </c>
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="2">
-        <v>42125</v>
-      </c>
-      <c r="G15" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="2">
-        <v>43891</v>
-      </c>
-      <c r="G16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="2">
-        <v>11383</v>
-      </c>
-      <c r="G17" t="s">
-        <v>25</v>
-      </c>
       <c r="H17" t="s">
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="F18" s="2">
-        <v>42125</v>
+        <v>11383</v>
       </c>
       <c r="G18" t="s">
         <v>25</v>
@@ -1398,48 +1411,51 @@
       <c r="H18" t="s">
         <v>10</v>
       </c>
-      <c r="I18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I18" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="F19" s="2">
-        <v>42125</v>
+        <v>42064</v>
       </c>
       <c r="G19" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H19" t="s">
         <v>10</v>
       </c>
-      <c r="I19" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I19" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>80</v>
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
       </c>
       <c r="D20" t="s">
         <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
       <c r="F20" s="2">
         <v>11383</v>
@@ -1448,18 +1464,18 @@
         <v>25</v>
       </c>
       <c r="H20" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="I20" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>84</v>
+      <c r="A21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" t="s">
+        <v>115</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
@@ -1468,599 +1484,698 @@
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>116</v>
       </c>
       <c r="F21" s="2">
-        <v>11444</v>
+        <v>42095</v>
       </c>
       <c r="G21" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="H21" t="s">
         <v>10</v>
       </c>
-      <c r="I21" t="s">
-        <v>85</v>
+      <c r="I21" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" t="s">
-        <v>20</v>
+      <c r="A22" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>128</v>
       </c>
       <c r="D22" t="s">
         <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>129</v>
       </c>
       <c r="F22" s="2">
-        <v>11383</v>
+        <v>42125</v>
       </c>
       <c r="G22" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="H22" t="s">
         <v>10</v>
       </c>
-      <c r="I22" t="s">
-        <v>52</v>
+      <c r="I22" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>92</v>
+      <c r="A23" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
       </c>
       <c r="D23" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>90</v>
+      <c r="E23" t="s">
+        <v>136</v>
       </c>
       <c r="F23" s="2">
-        <v>11049</v>
+        <v>42095</v>
       </c>
       <c r="G23" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="H23" t="s">
         <v>10</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>94</v>
+      <c r="A24" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
       </c>
       <c r="D24" t="s">
         <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="F24" s="2">
         <v>42125</v>
       </c>
       <c r="G24" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="H24" t="s">
         <v>17</v>
       </c>
       <c r="I24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" t="s">
-        <v>96</v>
-      </c>
-      <c r="F25" s="2">
-        <v>42125</v>
-      </c>
-      <c r="G25" t="s">
-        <v>65</v>
-      </c>
-      <c r="H25" t="s">
-        <v>10</v>
-      </c>
-      <c r="I25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" s="2">
-        <v>11383</v>
-      </c>
-      <c r="G26" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26" t="s">
-        <v>10</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" t="s">
-        <v>104</v>
-      </c>
-      <c r="F27" s="2">
-        <v>11383</v>
-      </c>
-      <c r="G27" t="s">
-        <v>25</v>
-      </c>
-      <c r="H27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D28" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28" s="2">
-        <v>11383</v>
-      </c>
-      <c r="G28" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" t="s">
-        <v>110</v>
-      </c>
-      <c r="F29" s="2">
-        <v>42064</v>
-      </c>
-      <c r="G29" t="s">
-        <v>25</v>
-      </c>
-      <c r="H29" t="s">
-        <v>10</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F30" s="2">
-        <v>42125</v>
-      </c>
-      <c r="G30" t="s">
-        <v>25</v>
-      </c>
-      <c r="H30" t="s">
-        <v>10</v>
-      </c>
-      <c r="I30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" t="s">
-        <v>114</v>
-      </c>
-      <c r="F31" s="2">
-        <v>11383</v>
-      </c>
-      <c r="G31" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>115</v>
-      </c>
-      <c r="B32" t="s">
-        <v>116</v>
-      </c>
-      <c r="C32" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" t="s">
-        <v>117</v>
-      </c>
-      <c r="F32" s="2">
-        <v>42095</v>
-      </c>
-      <c r="G32" t="s">
-        <v>25</v>
-      </c>
-      <c r="H32" t="s">
-        <v>10</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C33" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F33" s="2">
-        <v>11383</v>
-      </c>
-      <c r="G33" t="s">
-        <v>25</v>
-      </c>
-      <c r="H33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I33" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="C34" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" t="s">
-        <v>124</v>
-      </c>
-      <c r="F34" s="2">
-        <v>42125</v>
-      </c>
-      <c r="G34" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C35" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" t="s">
-        <v>36</v>
-      </c>
-      <c r="F35" s="2">
-        <v>42125</v>
-      </c>
-      <c r="G35" t="s">
-        <v>25</v>
-      </c>
-      <c r="H35" t="s">
-        <v>10</v>
-      </c>
-      <c r="I35" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D36" t="s">
-        <v>20</v>
-      </c>
-      <c r="E36" t="s">
-        <v>130</v>
-      </c>
-      <c r="F36" s="2">
-        <v>42125</v>
-      </c>
-      <c r="G36" t="s">
-        <v>25</v>
-      </c>
-      <c r="H36" t="s">
-        <v>10</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="D37" t="s">
-        <v>20</v>
-      </c>
-      <c r="E37" t="s">
-        <v>36</v>
-      </c>
-      <c r="F37" s="2">
-        <v>11383</v>
-      </c>
-      <c r="G37" t="s">
-        <v>25</v>
-      </c>
-      <c r="H37" t="s">
-        <v>10</v>
-      </c>
-      <c r="I37" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="C38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E38" t="s">
-        <v>137</v>
-      </c>
-      <c r="F38" s="2">
-        <v>42095</v>
-      </c>
-      <c r="G38" t="s">
-        <v>25</v>
-      </c>
-      <c r="H38" t="s">
-        <v>10</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="B39" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="C39" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" t="s">
-        <v>20</v>
-      </c>
-      <c r="E39" t="s">
-        <v>141</v>
-      </c>
-      <c r="F39" s="2">
-        <v>42125</v>
-      </c>
-      <c r="G39" t="s">
-        <v>65</v>
-      </c>
-      <c r="H39" t="s">
-        <v>17</v>
-      </c>
-      <c r="I39" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="C40" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40" t="s">
-        <v>20</v>
-      </c>
-      <c r="E40" t="s">
-        <v>143</v>
-      </c>
-      <c r="F40" s="2">
-        <v>42125</v>
-      </c>
-      <c r="G40" t="s">
-        <v>25</v>
-      </c>
-      <c r="H40" t="s">
-        <v>144</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="https://www.ismll.uni-hildesheim.de/da/index_en.html"/>
+    <hyperlink ref="I2" r:id="rId1"/>
     <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I5" r:id="rId3"/>
-    <hyperlink ref="I8" r:id="rId4"/>
-    <hyperlink ref="I23" r:id="rId5"/>
-    <hyperlink ref="E23" r:id="rId6"/>
-    <hyperlink ref="I27" r:id="rId7" display="http://www.uni-potsdam.de/en/studium/application-enrollment/application-master/consecutive.html,  "/>
-    <hyperlink ref="I26" r:id="rId8"/>
-    <hyperlink ref="I28" r:id="rId9"/>
-    <hyperlink ref="E30" r:id="rId10"/>
-    <hyperlink ref="I32" r:id="rId11"/>
-    <hyperlink ref="E33" r:id="rId12"/>
-    <hyperlink ref="I36" r:id="rId13"/>
-    <hyperlink ref="I38" r:id="rId14"/>
-    <hyperlink ref="I40" r:id="rId15"/>
+    <hyperlink ref="I15" r:id="rId3"/>
+    <hyperlink ref="E15" r:id="rId4"/>
+    <hyperlink ref="I18" r:id="rId5" display="http://www.uni-potsdam.de/en/studium/application-enrollment/application-master/consecutive.html,  "/>
+    <hyperlink ref="I21" r:id="rId6"/>
+    <hyperlink ref="I22" r:id="rId7"/>
+    <hyperlink ref="I23" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="146.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2">
+        <v>11049</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2">
+        <v>42125</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2">
+        <v>42125</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="2">
+        <v>11383</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" display="https://www.ismll.uni-hildesheim.de/da/index_en.html"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="135.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="152.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="2">
+        <v>11049</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2">
+        <v>11383</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="2">
+        <v>42125</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="2">
+        <v>11383</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="2">
+        <v>11383</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="2">
+        <v>11383</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="2">
+        <v>42125</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="2">
+        <v>11383</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="2">
+        <v>42125</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="2">
+        <v>42125</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I6" r:id="rId1"/>
+    <hyperlink ref="I7" r:id="rId2"/>
+    <hyperlink ref="E8" r:id="rId3"/>
+    <hyperlink ref="E9" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>